<commit_message>
add creating additional reports in Word
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="41490" windowHeight="16890" tabRatio="811" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="811" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="7" state="hidden" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="lov" sheetId="5" r:id="rId3"/>
     <sheet name="ФОРМА АВАНСОВОГО ОТЧЕТА &quot;АО-1&quot;" sheetId="1" state="hidden" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="89">
   <si>
     <t>Итого</t>
   </si>
@@ -1187,7 +1187,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,7 +1249,7 @@
       </c>
       <c r="C4" s="34">
         <f ca="1">TODAY()</f>
-        <v>45703</v>
+        <v>45706</v>
       </c>
       <c r="E4" t="s">
         <v>83</v>
@@ -1368,15 +1368,21 @@
       <c r="G8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1">
+        <v>4</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
@@ -1476,11 +1482,21 @@
         <v>41</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
@@ -1602,10 +1618,18 @@
       <c r="F15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -1631,10 +1655,18 @@
       <c r="F16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1660,10 +1692,18 @@
       <c r="F17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -1689,10 +1729,18 @@
       <c r="F18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -1718,10 +1766,18 @@
       <c r="F19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -1747,10 +1803,18 @@
       <c r="F20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -1776,10 +1840,18 @@
       <c r="F21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -1805,10 +1877,18 @@
       <c r="F22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -1834,10 +1914,18 @@
       <c r="F23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -1863,10 +1951,18 @@
       <c r="F24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -1907,13 +2003,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>lov!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>G18:G23</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>lov!$A:$A</xm:f>
@@ -2497,6 +2587,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d34705cf-da4a-477c-8c69-66639a86e9f8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Документ" ma:contentTypeID="0x0101003CB071791149854C89CD0E80DD6EE345" ma:contentTypeVersion="12" ma:contentTypeDescription="Создание документа." ma:contentTypeScope="" ma:versionID="7bf6f323435c7223df3e940e85a6bdc2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d34705cf-da4a-477c-8c69-66639a86e9f8" xmlns:ns4="547e0d17-6083-43b8-af57-983870e6b87e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c0033d975bd301c8b2a7aff1a5e881b2" ns3:_="" ns4:_="">
     <xsd:import namespace="d34705cf-da4a-477c-8c69-66639a86e9f8"/>
@@ -2711,24 +2818,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4675D14-1723-4358-9666-5A15D29D2D2A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="547e0d17-6083-43b8-af57-983870e6b87e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d34705cf-da4a-477c-8c69-66639a86e9f8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d34705cf-da4a-477c-8c69-66639a86e9f8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DC2FA73-190F-4087-93A3-B2D79B862635}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8C20107-FF3F-488E-9061-270EBC165AEB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2745,29 +2860,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DC2FA73-190F-4087-93A3-B2D79B862635}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4675D14-1723-4358-9666-5A15D29D2D2A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="547e0d17-6083-43b8-af57-983870e6b87e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="d34705cf-da4a-477c-8c69-66639a86e9f8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>